<commit_message>
SPR / DR shared
</commit_message>
<xml_diff>
--- a/resources/input/Trader Declaration Data 3.xlsx
+++ b/resources/input/Trader Declaration Data 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MLavis.Admin/sites and projects/1. Online Tariff/99. experiments/add code cds instructions/resources/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MLavis.Admin/sites and projects/1. Online Tariff/99. experiments/SPR excise code cds instructions/resources/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC469465-35D9-0F46-9BA2-40123564EEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4986CEFC-97E0-9049-9B5A-7840C59B350A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33220" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35120" yWindow="4800" windowWidth="31940" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Elements" sheetId="1" r:id="rId1"/>
@@ -37,159 +37,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="116">
   <si>
-    <t>Low Alcohol - not exc 1.2%</t>
-  </si>
-  <si>
     <t xml:space="preserve"> £                                  -   </t>
   </si>
   <si>
     <t>(litres x ABV%) x rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Beer less than 3.5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cider less than 3.5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wine less than 3.5% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other fermented products less than 3.5% </t>
-  </si>
-  <si>
-    <t>Spirits less than 3.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beer at least 3.5 but less than 8.5% </t>
-  </si>
-  <si>
-    <t>Cider at least 3.5 but less than 8.5% &amp; sparkling cider at least 3.5 not exceeding 5.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wine at least 3.5 but less than 8.5% </t>
-  </si>
-  <si>
-    <t>Other fermented products at least 3.5 but less than 8.5% &amp; sparkling cider exceeding 5.5 but less than 8.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirits at least 3.5 but less than 8.5% </t>
-  </si>
-  <si>
-    <t>Beer at least 8.5 but not exceeding 22%</t>
-  </si>
-  <si>
-    <t>Wine at least 8.5 but not exceeding 22%</t>
-  </si>
-  <si>
-    <t>Other fermented products at least 8.5 but not exceeding 22%</t>
-  </si>
-  <si>
-    <t>Spirits at least 8.5 but not exceeding 22%</t>
-  </si>
-  <si>
-    <t>Beer exceeding 22%</t>
-  </si>
-  <si>
-    <t>Wine exceeding 22%</t>
-  </si>
-  <si>
-    <t>Other fermented products exceeding 22%</t>
-  </si>
-  <si>
-    <t>Spirits exceeding 22%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beer less than 3.5% &amp; eligible for DR </t>
-  </si>
-  <si>
-    <t>Cider less than 3.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Wine less than 3.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Other fermented products less than 3.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Spirits less than 3.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Beer at least 3.5 but less than 8.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Cider at least 3.5 but less than 8.5% &amp; Sparkling cider at least 3.5 but less than not exceeding 5.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Wine at least 3.5 but less than 8.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Other fermented products at least 3.5 but less than 8.5% &amp; Sparkling cider exceeding 5.5 but less than 8.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Spirits at least 3.5 but less than 8.5% &amp; eligible for DR</t>
-  </si>
-  <si>
-    <t>Beer less than 3.5% &amp; eligible for SPR (small producer relief)</t>
-  </si>
-  <si>
-    <t>Cider less than 3.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Wine less than 3.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Other fermented products less than 3.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Spirits less than 3.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Beer at least 3.5 but less than 8.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Cider at least 3.5 but less than 8.5% &amp; Sparkling cider at least 3.5 but less than not exceeding 5.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Wine at least 3.5 but less than 8.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Other fermented products at least 3.5 but less than 8.5% &amp; Sparkling cider exceeding 5.5 but less than 8.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Spirits at least 3.5 but less than 8.5% &amp; eligible for SPR</t>
-  </si>
-  <si>
-    <t>Beer less than 3.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Cider less than 3.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Wine less than 3.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Other fermented products less than 3.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Spirits less than 3.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Beer at least 3.5 but less than 8.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Cider at least 3.5 but less than 8.5% &amp; Sparkling cider at least 3.5 but less than not exceeding 5.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Wine at least 3.5 but less than 8.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Other fermented products at least 3.5 but less than 8.5% &amp; Sparkling cider exceeding 5.5 but less than 8.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
-    <t>Spirits at least 3.5 but less than 8.5% &amp; eligible for SPR and DR</t>
-  </si>
-  <si>
     <t>Must be Equal to or Under 1.2%</t>
   </si>
   <si>
@@ -383,6 +236,153 @@
   </si>
   <si>
     <t>Only if tariff mandates</t>
+  </si>
+  <si>
+    <t>spirits at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>low alcohol products, with an ABV not exceeding 1.2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer with an ABV less than 3.5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cider with an ABV less than 3.5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wine with an ABV less than 3.5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">other fermented products with an ABV less than 3.5% </t>
+  </si>
+  <si>
+    <t>spirits with an ABV less than 3.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer with an ABV at least 3.5% but less than 8.5% </t>
+  </si>
+  <si>
+    <t>cider with an ABV at least 3.5% but less than 8.5% and sparkling cider with an ABV at least 3.5% not exceeding 5.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wine with an ABV at least 3.5% but less than 8.5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">spirits with an ABV at least 3.5% but less than 8.5% </t>
+  </si>
+  <si>
+    <t>beer with an ABV at least 8.5% but not exceeding 22%</t>
+  </si>
+  <si>
+    <t>wine with an ABV at least 8.5% but not exceeding 22%</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV at least 8.5% but not exceeding 22%</t>
+  </si>
+  <si>
+    <t>spirits with an ABV at least 8.5% but not exceeding 22%</t>
+  </si>
+  <si>
+    <t>beer with an ABV exceeding 22%</t>
+  </si>
+  <si>
+    <t>wine with an ABV exceeding 22%</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV exceeding 22%</t>
+  </si>
+  <si>
+    <t>spirits with an ABV exceeding 22%</t>
+  </si>
+  <si>
+    <t>beer with an ABV less than 3.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV less than 3.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV less than 3.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV less than 3.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>spirits with an ABV less than 3.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>beer with an ABV at least 3.5% but less than 8.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV at least 3.5% but less than 8.5% and sparkling cider with an ABV at least 3.5% but less than not exceeding 5.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV at least 3.5% but less than 8.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV at least 3.5% but less than 8.5% and sparkling cider exceeding 5.5% but less than 8.5%</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV at least 3.5% but less than 8.5% and sparkling cider with an ABV exceeding 5.5% but less than 8.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>spirits with an ABV at least 3.5% but less than 8.5% and eligible for DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>beer with an ABV less than 3.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV less than 3.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV less than 3.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV less than 3.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>spirits with an ABV less than 3.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>beer with an ABV at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV at least 3.5% but less than 8.5% and Sparkling cider at least 3.5% but less than not exceeding 5.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV at least 3.5% but less than 8.5% and sparkling cider with an ABV exceeding 5.5% but less than 8.5% and eligible for SPR (Small Producer Relief)</t>
+  </si>
+  <si>
+    <t>beer with an ABV less than 3.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV less than 3.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV less than 3.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV less than 3.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>spirits with an ABV less than 3.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>beer with an ABV at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>cider with an ABV at least 3.5% but less than 8.5% and Sparkling cider at least 3.5% but less than not exceeding 5.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>wine with an ABV at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>other fermented products with an ABV at least 3.5% but less than 8.5% and sparkling cider with an ABV exceeding 5.5% but less than 8.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
+  </si>
+  <si>
+    <t>spirits with an ABV at least 3.5% but less than 8.5% and eligible for SPR (Small Producer Relief) and DR (Draught Relief)</t>
   </si>
 </sst>
 </file>
@@ -859,15 +859,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="110.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="146.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="13"/>
     <col min="5" max="5" width="10.33203125" style="13" customWidth="1"/>
@@ -888,43 +888,43 @@
         <v>301</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="15">
         <v>301</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -932,43 +932,43 @@
         <v>311</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3">
         <v>9.27</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="13">
         <v>311</v>
       </c>
       <c r="F2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="K2" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -976,43 +976,43 @@
         <v>312</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3">
         <v>9.27</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="13">
         <v>312</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,43 +1020,43 @@
         <v>313</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C4" s="8">
         <v>9.27</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="15">
         <v>313</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1064,43 +1064,43 @@
         <v>314</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C5" s="8">
         <v>9.27</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="15">
         <v>314</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1108,43 +1108,43 @@
         <v>315</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C6" s="8">
         <v>9.27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="15">
         <v>315</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1152,43 +1152,43 @@
         <v>321</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3">
         <v>21.01</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="13">
         <v>321</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1196,43 +1196,43 @@
         <v>322</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3">
         <v>9.67</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="13">
         <v>322</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1240,43 +1240,43 @@
         <v>323</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C9" s="8">
         <v>24.77</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="15">
         <v>323</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1284,43 +1284,43 @@
         <v>324</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="C10" s="3">
         <v>24.77</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="13">
         <v>324</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1328,43 +1328,43 @@
         <v>325</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="C11" s="8">
         <v>24.77</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="15">
         <v>325</v>
       </c>
       <c r="F11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>112</v>
-      </c>
       <c r="H11" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1372,43 +1372,43 @@
         <v>331</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="C12" s="3">
         <v>28.5</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="13">
         <v>331</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1416,43 +1416,43 @@
         <v>333</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3">
         <v>28.5</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="13">
         <v>333</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1460,43 +1460,43 @@
         <v>334</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3">
         <v>28.5</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="13">
         <v>334</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1504,43 +1504,43 @@
         <v>335</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C15" s="8">
         <v>28.5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="15">
         <v>335</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1548,43 +1548,43 @@
         <v>341</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3">
         <v>31.64</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="13">
         <v>341</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1592,43 +1592,43 @@
         <v>343</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C17" s="3">
         <v>31.64</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="13">
         <v>343</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1636,43 +1636,43 @@
         <v>344</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C18" s="3">
         <v>31.64</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="13">
         <v>344</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1680,43 +1680,43 @@
         <v>345</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="C19" s="8">
         <v>31.64</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="15">
         <v>345</v>
       </c>
       <c r="F19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="N19" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="L19" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1724,43 +1724,43 @@
         <v>351</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3">
         <v>8.42</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="13">
         <v>351</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1768,43 +1768,43 @@
         <v>352</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="C21" s="3">
         <v>8.42</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="13">
         <v>352</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,43 +1812,43 @@
         <v>353</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="C22" s="8">
         <v>8.42</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="15">
         <v>353</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1856,43 +1856,43 @@
         <v>354</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="C23" s="8">
         <v>8.42</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="15">
         <v>354</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1900,43 +1900,43 @@
         <v>355</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C24" s="3">
         <v>8.42</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="13">
         <v>355</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1944,43 +1944,43 @@
         <v>356</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="C25" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="13">
         <v>356</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1988,43 +1988,43 @@
         <v>357</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3">
         <v>8.7799999999999994</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="13">
         <v>357</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2032,43 +2032,43 @@
         <v>358</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C27" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="13">
         <v>358</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2076,43 +2076,43 @@
         <v>359</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C28" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="13">
         <v>359</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N28" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2120,43 +2120,43 @@
         <v>360</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C29" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="13">
         <v>360</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N29" s="13" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2164,43 +2164,43 @@
         <v>361</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C30" s="3">
         <v>9.27</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="13">
         <v>361</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2208,43 +2208,43 @@
         <v>362</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C31" s="3">
         <v>9.27</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="13">
         <v>362</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M31" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2252,43 +2252,43 @@
         <v>363</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C32" s="3">
         <v>9.27</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="13">
         <v>363</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2296,43 +2296,43 @@
         <v>364</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="C33" s="3">
         <v>9.27</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="13">
         <v>364</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M33" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N33" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2340,43 +2340,43 @@
         <v>365</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="C34" s="3">
         <v>9.27</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="13">
         <v>365</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2384,43 +2384,43 @@
         <v>366</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="C35" s="3">
         <v>21.01</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="13">
         <v>366</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N35" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2428,43 +2428,43 @@
         <v>367</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C36" s="3">
         <v>9.67</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="13">
         <v>367</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M36" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2472,43 +2472,43 @@
         <v>368</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C37" s="3">
         <v>24.77</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="13">
         <v>368</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2516,43 +2516,43 @@
         <v>369</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="C38" s="3">
         <v>24.77</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="13">
         <v>369</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N38" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2560,43 +2560,43 @@
         <v>370</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C39" s="3">
         <v>24.77</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="13">
         <v>370</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N39" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2604,43 +2604,43 @@
         <v>371</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="C40" s="3">
         <v>8.42</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="13">
         <v>371</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N40" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2648,43 +2648,43 @@
         <v>372</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="C41" s="3">
         <v>8.42</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="13">
         <v>372</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2692,43 +2692,43 @@
         <v>373</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="C42" s="3">
         <v>8.42</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="13">
         <v>373</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2736,43 +2736,43 @@
         <v>374</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="C43" s="11">
         <v>8.42</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="18">
         <v>374</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2780,43 +2780,43 @@
         <v>375</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C44" s="11">
         <v>8.42</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="18">
         <v>375</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2824,43 +2824,43 @@
         <v>376</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="C45" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" s="13">
         <v>376</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2868,43 +2868,43 @@
         <v>377</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="C46" s="3">
         <v>8.7799999999999994</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="13">
         <v>377</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2912,43 +2912,43 @@
         <v>378</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C47" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="13">
         <v>378</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N47" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2956,43 +2956,43 @@
         <v>379</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="C48" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" s="13">
         <v>379</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N48" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3000,43 +3000,43 @@
         <v>380</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="C49" s="3">
         <v>19.079999999999998</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="13">
         <v>380</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="M49" s="12" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>